<commit_message>
Merge cells in the output table
</commit_message>
<xml_diff>
--- a/SERCO-TUG/results.xlsx
+++ b/SERCO-TUG/results.xlsx
@@ -59,12 +59,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -2271,6 +2274,17 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13" customWidth="1" style="3" min="1" max="1"/>
+    <col width="13" customWidth="1" style="3" min="2" max="2"/>
+    <col width="13" customWidth="1" style="3" min="3" max="3"/>
+    <col width="13" customWidth="1" style="3" min="4" max="4"/>
+    <col width="13" customWidth="1" style="3" min="5" max="5"/>
+    <col width="13" customWidth="1" style="3" min="6" max="6"/>
+    <col width="13" customWidth="1" style="3" min="8" max="8"/>
+    <col width="13" customWidth="1" style="3" min="9" max="9"/>
+    <col width="13" customWidth="1" style="3" min="10" max="10"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
@@ -2328,10 +2342,10 @@
       <c r="G2" t="n">
         <v>169.2873122388889</v>
       </c>
-      <c r="H2.0" t="n">
+      <c r="H2" t="n">
         <v>0</v>
       </c>
-      <c r="I2.0" t="n">
+      <c r="I2" t="n">
         <v>235.3797588068789</v>
       </c>
     </row>
@@ -2361,6 +2375,12 @@
       <c r="G3" t="n">
         <v>110.3666201713889</v>
       </c>
+      <c r="H3.0" t="n">
+        <v>19.96308</v>
+      </c>
+      <c r="I3.0" t="n">
+        <v>598.2789926021113</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -2368,11 +2388,6 @@
           <t>Trip 3</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>02-02</t>
-        </is>
-      </c>
       <c r="C4" t="n">
         <v>0.2774997222222222</v>
       </c>
@@ -2395,11 +2410,6 @@
           <t>Trip 4</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>02-02</t>
-        </is>
-      </c>
       <c r="C5" t="n">
         <v>1.811111111111111</v>
       </c>
@@ -2422,11 +2432,6 @@
           <t>Trip 5</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>02-02</t>
-        </is>
-      </c>
       <c r="C6" t="n">
         <v>1.318611111111111</v>
       </c>
@@ -2469,6 +2474,12 @@
       <c r="G7" t="n">
         <v>428.2980651725</v>
       </c>
+      <c r="H7.0" t="n">
+        <v>15.29562527777778</v>
+      </c>
+      <c r="I7.0" t="n">
+        <v>511.5087740618281</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -2476,11 +2487,6 @@
           <t>Trip 7</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>03-02</t>
-        </is>
-      </c>
       <c r="C8" t="n">
         <v>0.5311105555555555</v>
       </c>
@@ -2523,6 +2529,12 @@
       <c r="G9" t="n">
         <v>132.9426997233333</v>
       </c>
+      <c r="H9.0" t="n">
+        <v>23.83664055555556</v>
+      </c>
+      <c r="I9.0" t="n">
+        <v>500.168620007151</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -2530,11 +2542,6 @@
           <t>Trip 10</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>04-02</t>
-        </is>
-      </c>
       <c r="C10" t="n">
         <v>2.885555555555555</v>
       </c>
@@ -2557,11 +2564,6 @@
           <t>Trip 11</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>04-02</t>
-        </is>
-      </c>
       <c r="C11" t="n">
         <v>0.2494444444444444</v>
       </c>
@@ -2604,6 +2606,12 @@
       <c r="G12" t="n">
         <v>169.3884568372222</v>
       </c>
+      <c r="H12.0" t="n">
+        <v>13.92822055555555</v>
+      </c>
+      <c r="I12.0" t="n">
+        <v>448.4274068557453</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -2631,6 +2639,12 @@
       <c r="G13" t="n">
         <v>124.5344426672222</v>
       </c>
+      <c r="H13.0" t="n">
+        <v>22.24077194444444</v>
+      </c>
+      <c r="I13.0" t="n">
+        <v>208.3632598934118</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -2658,6 +2672,12 @@
       <c r="G14" t="n">
         <v>193.5261132388889</v>
       </c>
+      <c r="H14.0" t="n">
+        <v>21.35485166666667</v>
+      </c>
+      <c r="I14.0" t="n">
+        <v>472.0041050347856</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -2685,6 +2705,12 @@
       <c r="G15" t="n">
         <v>93.23065847333334</v>
       </c>
+      <c r="H15.0" t="n">
+        <v>29.43345861111111</v>
+      </c>
+      <c r="I15.0" t="n">
+        <v>145.5463991936819</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -2712,6 +2738,12 @@
       <c r="G16" t="n">
         <v>193.8882349988889</v>
       </c>
+      <c r="H16.0" t="n">
+        <v>23.54935666666667</v>
+      </c>
+      <c r="I16.0" t="n">
+        <v>1005.847775626425</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -2719,11 +2751,6 @@
           <t>Trip 18</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>12-02</t>
-        </is>
-      </c>
       <c r="C17" t="n">
         <v>0.7297219444444445</v>
       </c>
@@ -2746,11 +2773,6 @@
           <t>Trip 19</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>12-02</t>
-        </is>
-      </c>
       <c r="C18" t="n">
         <v>1.94</v>
       </c>
@@ -2793,6 +2815,12 @@
       <c r="G19" t="n">
         <v>70.25490951666666</v>
       </c>
+      <c r="H19.0" t="n">
+        <v>14.47349555555556</v>
+      </c>
+      <c r="I19.0" t="n">
+        <v>41.85755292711956</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -2820,6 +2848,12 @@
       <c r="G20" t="n">
         <v>238.2769932538889</v>
       </c>
+      <c r="H20.0" t="n">
+        <v>23.85865527777778</v>
+      </c>
+      <c r="I20.0" t="n">
+        <v>457.8345346310019</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -2847,6 +2881,12 @@
       <c r="G21" t="n">
         <v>61.92750327527778</v>
       </c>
+      <c r="H21.0" t="n">
+        <v>28.16782055555555</v>
+      </c>
+      <c r="I21.0" t="n">
+        <v>894.9659266487342</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -2854,11 +2894,6 @@
           <t>Trip 27</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>19-02</t>
-        </is>
-      </c>
       <c r="C22" t="n">
         <v>0.7794452777777777</v>
       </c>
@@ -2881,11 +2916,6 @@
           <t>Trip 28</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>19-02</t>
-        </is>
-      </c>
       <c r="C23" t="n">
         <v>2.109999722222222</v>
       </c>
@@ -2928,6 +2958,12 @@
       <c r="G24" t="n">
         <v>54.74240011638889</v>
       </c>
+      <c r="H24.0" t="n">
+        <v>10.78825</v>
+      </c>
+      <c r="I24.0" t="n">
+        <v>234.515397511714</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -2935,11 +2971,6 @@
           <t>Trip 30</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>20-02</t>
-        </is>
-      </c>
       <c r="C25" t="n">
         <v>2.001383888888889</v>
       </c>
@@ -2982,6 +3013,12 @@
       <c r="G26" t="n">
         <v>269.733323215</v>
       </c>
+      <c r="H26.0" t="n">
+        <v>22.06193444444444</v>
+      </c>
+      <c r="I26.0" t="n">
+        <v>703.2983644786177</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -2989,11 +3026,6 @@
           <t>Trip 33</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>22-02</t>
-        </is>
-      </c>
       <c r="C27" t="n">
         <v>0.2830552777777778</v>
       </c>
@@ -3016,11 +3048,6 @@
           <t>Trip 34</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>22-02</t>
-        </is>
-      </c>
       <c r="C28" t="n">
         <v>0.9827777777777778</v>
       </c>
@@ -3063,6 +3090,12 @@
       <c r="G29" t="n">
         <v>138.0112086555555</v>
       </c>
+      <c r="H29.0" t="n">
+        <v>18.60271083333333</v>
+      </c>
+      <c r="I29.0" t="n">
+        <v>513.7033494652303</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -3070,11 +3103,6 @@
           <t>Trip 36</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>23-02</t>
-        </is>
-      </c>
       <c r="C30" t="n">
         <v>1.535556111111111</v>
       </c>
@@ -3117,6 +3145,12 @@
       <c r="G31" t="n">
         <v>308.7708649383333</v>
       </c>
+      <c r="H31.0" t="n">
+        <v>23.90431666666667</v>
+      </c>
+      <c r="I31.0" t="n">
+        <v>798.1247673398506</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -3124,11 +3158,6 @@
           <t>Trip 38</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>24-02</t>
-        </is>
-      </c>
       <c r="C32" t="n">
         <v>0.865</v>
       </c>
@@ -3151,11 +3180,6 @@
           <t>Trip 39</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>24-02</t>
-        </is>
-      </c>
       <c r="C33" t="n">
         <v>1.302222222222222</v>
       </c>
@@ -3198,6 +3222,12 @@
       <c r="G34" t="n">
         <v>158.358051665</v>
       </c>
+      <c r="H34.0" t="n">
+        <v>18.45900277777778</v>
+      </c>
+      <c r="I34.0" t="n">
+        <v>518.7885898847807</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -3205,11 +3235,6 @@
           <t>Trip 41</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>25-02</t>
-        </is>
-      </c>
       <c r="C35" t="n">
         <v>0.2769441666666667</v>
       </c>
@@ -3232,11 +3257,6 @@
           <t>Trip 42</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>25-02</t>
-        </is>
-      </c>
       <c r="C36" t="n">
         <v>0.3702777777777778</v>
       </c>
@@ -3259,11 +3279,6 @@
           <t>Trip 43</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>25-02</t>
-        </is>
-      </c>
       <c r="C37" t="n">
         <v>1.1722225</v>
       </c>
@@ -3286,11 +3301,6 @@
           <t>Trip 44</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>25-02</t>
-        </is>
-      </c>
       <c r="C38" t="n">
         <v>0.4225</v>
       </c>
@@ -3333,6 +3343,12 @@
       <c r="G39" t="n">
         <v>136.5821605008333</v>
       </c>
+      <c r="H39.0" t="n">
+        <v>16.43696861111111</v>
+      </c>
+      <c r="I39.0" t="n">
+        <v>283.4538369956304</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -3340,11 +3356,6 @@
           <t>Trip 46</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>26-02</t>
-        </is>
-      </c>
       <c r="C40" t="n">
         <v>1.078055</v>
       </c>
@@ -3362,43 +3373,61 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="54">
+    <mergeCell ref="B2"/>
     <mergeCell ref="H2"/>
     <mergeCell ref="I2"/>
-    <mergeCell ref="H2:H6"/>
-    <mergeCell ref="I2:I6"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="I6:I8"/>
-    <mergeCell ref="H8:H11"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="H25:H28"/>
-    <mergeCell ref="I25:I28"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="I30:I33"/>
-    <mergeCell ref="H33:H38"/>
-    <mergeCell ref="I33:I38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="H3:H6"/>
+    <mergeCell ref="I3:I6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="B12"/>
+    <mergeCell ref="H12"/>
+    <mergeCell ref="I12"/>
+    <mergeCell ref="B13"/>
+    <mergeCell ref="H13"/>
+    <mergeCell ref="I13"/>
+    <mergeCell ref="B14"/>
+    <mergeCell ref="H14"/>
+    <mergeCell ref="I14"/>
+    <mergeCell ref="B15"/>
+    <mergeCell ref="H15"/>
+    <mergeCell ref="I15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="B19"/>
+    <mergeCell ref="H19"/>
+    <mergeCell ref="I19"/>
+    <mergeCell ref="B20"/>
+    <mergeCell ref="H20"/>
+    <mergeCell ref="I20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="I26:I28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="H31:H33"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="H34:H38"/>
+    <mergeCell ref="I34:I38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="I39:I40"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>